<commit_message>
added test for regular user, divided sucess and fail tests
</commit_message>
<xml_diff>
--- a/tests/downloads/moderation_events.xlsx
+++ b/tests/downloads/moderation_events.xlsx
@@ -474,7 +474,7 @@
         <v>PENDING</v>
       </c>
       <c r="G3" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H3" t="str">
         <v>April 29, 2025</v>
@@ -708,7 +708,7 @@
         <v>PENDING</v>
       </c>
       <c r="G12" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H12" t="str">
         <v>April 28, 2025</v>
@@ -734,7 +734,7 @@
         <v>PENDING</v>
       </c>
       <c r="G13" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H13" t="str">
         <v>April 28, 2025</v>
@@ -760,7 +760,7 @@
         <v>PENDING</v>
       </c>
       <c r="G14" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H14" t="str">
         <v>April 25, 2025</v>
@@ -786,7 +786,7 @@
         <v>PENDING</v>
       </c>
       <c r="G15" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H15" t="str">
         <v>April 25, 2025</v>
@@ -812,7 +812,7 @@
         <v>PENDING</v>
       </c>
       <c r="G16" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H16" t="str">
         <v>April 25, 2025</v>
@@ -838,7 +838,7 @@
         <v>PENDING</v>
       </c>
       <c r="G17" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H17" t="str">
         <v>April 24, 2025</v>
@@ -864,7 +864,7 @@
         <v>PENDING</v>
       </c>
       <c r="G18" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H18" t="str">
         <v>April 24, 2025</v>
@@ -890,7 +890,7 @@
         <v>PENDING</v>
       </c>
       <c r="G19" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H19" t="str">
         <v>April 24, 2025</v>
@@ -916,7 +916,7 @@
         <v>PENDING</v>
       </c>
       <c r="G20" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H20" t="str">
         <v>April 24, 2025</v>
@@ -942,7 +942,7 @@
         <v>PENDING</v>
       </c>
       <c r="G21" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H21" t="str">
         <v>April 24, 2025</v>
@@ -968,7 +968,7 @@
         <v>PENDING</v>
       </c>
       <c r="G22" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H22" t="str">
         <v>April 24, 2025</v>
@@ -994,7 +994,7 @@
         <v>PENDING</v>
       </c>
       <c r="G23" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H23" t="str">
         <v>April 24, 2025</v>
@@ -1020,7 +1020,7 @@
         <v>PENDING</v>
       </c>
       <c r="G24" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H24" t="str">
         <v>April 24, 2025</v>
@@ -1046,7 +1046,7 @@
         <v>PENDING</v>
       </c>
       <c r="G25" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H25" t="str">
         <v>April 24, 2025</v>
@@ -1072,7 +1072,7 @@
         <v>PENDING</v>
       </c>
       <c r="G26" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H26" t="str">
         <v>April 24, 2025</v>
@@ -1098,7 +1098,7 @@
         <v>PENDING</v>
       </c>
       <c r="G27" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H27" t="str">
         <v>April 24, 2025</v>
@@ -1124,7 +1124,7 @@
         <v>PENDING</v>
       </c>
       <c r="G28" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H28" t="str">
         <v>April 24, 2025</v>
@@ -1150,7 +1150,7 @@
         <v>PENDING</v>
       </c>
       <c r="G29" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H29" t="str">
         <v>April 24, 2025</v>
@@ -1176,7 +1176,7 @@
         <v>PENDING</v>
       </c>
       <c r="G30" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H30" t="str">
         <v>April 24, 2025</v>
@@ -1202,7 +1202,7 @@
         <v>PENDING</v>
       </c>
       <c r="G31" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H31" t="str">
         <v>April 24, 2025</v>
@@ -1228,7 +1228,7 @@
         <v>PENDING</v>
       </c>
       <c r="G32" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H32" t="str">
         <v>April 24, 2025</v>
@@ -1254,7 +1254,7 @@
         <v>PENDING</v>
       </c>
       <c r="G33" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H33" t="str">
         <v>April 24, 2025</v>
@@ -1280,7 +1280,7 @@
         <v>PENDING</v>
       </c>
       <c r="G34" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H34" t="str">
         <v>April 24, 2025</v>
@@ -1306,7 +1306,7 @@
         <v>PENDING</v>
       </c>
       <c r="G35" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H35" t="str">
         <v>April 24, 2025</v>
@@ -1332,7 +1332,7 @@
         <v>PENDING</v>
       </c>
       <c r="G36" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H36" t="str">
         <v>April 24, 2025</v>
@@ -1358,7 +1358,7 @@
         <v>PENDING</v>
       </c>
       <c r="G37" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H37" t="str">
         <v>April 24, 2025</v>
@@ -1384,7 +1384,7 @@
         <v>PENDING</v>
       </c>
       <c r="G38" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H38" t="str">
         <v>April 24, 2025</v>
@@ -1410,7 +1410,7 @@
         <v>PENDING</v>
       </c>
       <c r="G39" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H39" t="str">
         <v>April 24, 2025</v>
@@ -1436,7 +1436,7 @@
         <v>PENDING</v>
       </c>
       <c r="G40" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H40" t="str">
         <v>April 24, 2025</v>
@@ -1462,7 +1462,7 @@
         <v>PENDING</v>
       </c>
       <c r="G41" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H41" t="str">
         <v>April 24, 2025</v>
@@ -1488,7 +1488,7 @@
         <v>PENDING</v>
       </c>
       <c r="G42" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H42" t="str">
         <v>April 24, 2025</v>
@@ -1618,7 +1618,7 @@
         <v>PENDING</v>
       </c>
       <c r="G47" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H47" t="str">
         <v>April 23, 2025</v>
@@ -1644,7 +1644,7 @@
         <v>PENDING</v>
       </c>
       <c r="G48" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H48" t="str">
         <v>April 23, 2025</v>
@@ -1670,7 +1670,7 @@
         <v>PENDING</v>
       </c>
       <c r="G49" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H49" t="str">
         <v>April 23, 2025</v>
@@ -1696,7 +1696,7 @@
         <v>PENDING</v>
       </c>
       <c r="G50" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H50" t="str">
         <v>April 23, 2025</v>
@@ -1722,7 +1722,7 @@
         <v>PENDING</v>
       </c>
       <c r="G51" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H51" t="str">
         <v>April 23, 2025</v>
@@ -1748,7 +1748,7 @@
         <v>PENDING</v>
       </c>
       <c r="G52" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H52" t="str">
         <v>April 23, 2025</v>
@@ -1774,7 +1774,7 @@
         <v>PENDING</v>
       </c>
       <c r="G53" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H53" t="str">
         <v>April 23, 2025</v>
@@ -1800,7 +1800,7 @@
         <v>PENDING</v>
       </c>
       <c r="G54" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H54" t="str">
         <v>April 23, 2025</v>
@@ -1826,7 +1826,7 @@
         <v>PENDING</v>
       </c>
       <c r="G55" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H55" t="str">
         <v>April 23, 2025</v>
@@ -1852,7 +1852,7 @@
         <v>PENDING</v>
       </c>
       <c r="G56" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H56" t="str">
         <v>April 23, 2025</v>
@@ -1878,7 +1878,7 @@
         <v>PENDING</v>
       </c>
       <c r="G57" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H57" t="str">
         <v>April 23, 2025</v>
@@ -1904,7 +1904,7 @@
         <v>PENDING</v>
       </c>
       <c r="G58" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H58" t="str">
         <v>April 23, 2025</v>
@@ -1930,7 +1930,7 @@
         <v>PENDING</v>
       </c>
       <c r="G59" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H59" t="str">
         <v>April 23, 2025</v>
@@ -1956,7 +1956,7 @@
         <v>PENDING</v>
       </c>
       <c r="G60" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H60" t="str">
         <v>April 23, 2025</v>
@@ -1982,7 +1982,7 @@
         <v>PENDING</v>
       </c>
       <c r="G61" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H61" t="str">
         <v>April 23, 2025</v>
@@ -2060,7 +2060,7 @@
         <v>PENDING</v>
       </c>
       <c r="G64" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H64" t="str">
         <v>April 22, 2025</v>
@@ -2086,7 +2086,7 @@
         <v>PENDING</v>
       </c>
       <c r="G65" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H65" t="str">
         <v>April 22, 2025</v>
@@ -2112,7 +2112,7 @@
         <v>PENDING</v>
       </c>
       <c r="G66" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H66" t="str">
         <v>April 22, 2025</v>
@@ -2138,7 +2138,7 @@
         <v>PENDING</v>
       </c>
       <c r="G67" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H67" t="str">
         <v>April 22, 2025</v>
@@ -2164,7 +2164,7 @@
         <v>PENDING</v>
       </c>
       <c r="G68" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H68" t="str">
         <v>April 22, 2025</v>
@@ -2190,7 +2190,7 @@
         <v>PENDING</v>
       </c>
       <c r="G69" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H69" t="str">
         <v>April 22, 2025</v>
@@ -2216,7 +2216,7 @@
         <v>PENDING</v>
       </c>
       <c r="G70" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H70" t="str">
         <v>April 22, 2025</v>
@@ -2242,7 +2242,7 @@
         <v>PENDING</v>
       </c>
       <c r="G71" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H71" t="str">
         <v>April 22, 2025</v>
@@ -2268,7 +2268,7 @@
         <v>PENDING</v>
       </c>
       <c r="G72" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H72" t="str">
         <v>April 22, 2025</v>
@@ -2294,7 +2294,7 @@
         <v>PENDING</v>
       </c>
       <c r="G73" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H73" t="str">
         <v>April 22, 2025</v>
@@ -2320,7 +2320,7 @@
         <v>PENDING</v>
       </c>
       <c r="G74" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H74" t="str">
         <v>April 22, 2025</v>
@@ -2346,7 +2346,7 @@
         <v>PENDING</v>
       </c>
       <c r="G75" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H75" t="str">
         <v>April 21, 2025</v>
@@ -2372,7 +2372,7 @@
         <v>PENDING</v>
       </c>
       <c r="G76" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H76" t="str">
         <v>April 21, 2025</v>
@@ -2398,7 +2398,7 @@
         <v>PENDING</v>
       </c>
       <c r="G77" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H77" t="str">
         <v>April 21, 2025</v>
@@ -2476,7 +2476,7 @@
         <v>PENDING</v>
       </c>
       <c r="G80" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H80" t="str">
         <v>April 21, 2025</v>
@@ -2502,7 +2502,7 @@
         <v>PENDING</v>
       </c>
       <c r="G81" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H81" t="str">
         <v>April 21, 2025</v>
@@ -2528,7 +2528,7 @@
         <v>PENDING</v>
       </c>
       <c r="G82" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H82" t="str">
         <v>April 20, 2025</v>
@@ -2580,7 +2580,7 @@
         <v>PENDING</v>
       </c>
       <c r="G84" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H84" t="str">
         <v>April 19, 2025</v>
@@ -2606,7 +2606,7 @@
         <v>PENDING</v>
       </c>
       <c r="G85" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H85" t="str">
         <v>April 19, 2025</v>
@@ -2658,7 +2658,7 @@
         <v>PENDING</v>
       </c>
       <c r="G87" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H87" t="str">
         <v>April 19, 2025</v>
@@ -2814,7 +2814,7 @@
         <v>PENDING</v>
       </c>
       <c r="G93" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H93" t="str">
         <v>April 18, 2025</v>
@@ -2840,7 +2840,7 @@
         <v>PENDING</v>
       </c>
       <c r="G94" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H94" t="str">
         <v>April 18, 2025</v>
@@ -2866,7 +2866,7 @@
         <v>PENDING</v>
       </c>
       <c r="G95" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H95" t="str">
         <v>April 18, 2025</v>
@@ -2918,7 +2918,7 @@
         <v>PENDING</v>
       </c>
       <c r="G97" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H97" t="str">
         <v>April 18, 2025</v>
@@ -2944,7 +2944,7 @@
         <v>PENDING</v>
       </c>
       <c r="G98" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H98" t="str">
         <v>April 18, 2025</v>
@@ -2996,7 +2996,7 @@
         <v>PENDING</v>
       </c>
       <c r="G100" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H100" t="str">
         <v>April 18, 2025</v>
@@ -3022,7 +3022,7 @@
         <v>PENDING</v>
       </c>
       <c r="G101" t="str">
-        <v>April 30, 2025</v>
+        <v>May 1, 2025</v>
       </c>
       <c r="H101" t="str">
         <v>April 18, 2025</v>

</xml_diff>

<commit_message>
replaced quotes with double quotes
</commit_message>
<xml_diff>
--- a/tests/downloads/moderation_events.xlsx
+++ b/tests/downloads/moderation_events.xlsx
@@ -474,7 +474,7 @@
         <v>PENDING</v>
       </c>
       <c r="G3" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H3" t="str">
         <v>April 29, 2025</v>
@@ -708,7 +708,7 @@
         <v>PENDING</v>
       </c>
       <c r="G12" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H12" t="str">
         <v>April 28, 2025</v>
@@ -734,7 +734,7 @@
         <v>PENDING</v>
       </c>
       <c r="G13" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H13" t="str">
         <v>April 28, 2025</v>
@@ -760,7 +760,7 @@
         <v>PENDING</v>
       </c>
       <c r="G14" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H14" t="str">
         <v>April 25, 2025</v>
@@ -786,7 +786,7 @@
         <v>PENDING</v>
       </c>
       <c r="G15" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H15" t="str">
         <v>April 25, 2025</v>
@@ -812,7 +812,7 @@
         <v>PENDING</v>
       </c>
       <c r="G16" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H16" t="str">
         <v>April 25, 2025</v>
@@ -838,7 +838,7 @@
         <v>PENDING</v>
       </c>
       <c r="G17" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H17" t="str">
         <v>April 24, 2025</v>
@@ -864,7 +864,7 @@
         <v>PENDING</v>
       </c>
       <c r="G18" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H18" t="str">
         <v>April 24, 2025</v>
@@ -890,7 +890,7 @@
         <v>PENDING</v>
       </c>
       <c r="G19" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H19" t="str">
         <v>April 24, 2025</v>
@@ -916,7 +916,7 @@
         <v>PENDING</v>
       </c>
       <c r="G20" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H20" t="str">
         <v>April 24, 2025</v>
@@ -942,7 +942,7 @@
         <v>PENDING</v>
       </c>
       <c r="G21" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H21" t="str">
         <v>April 24, 2025</v>
@@ -968,7 +968,7 @@
         <v>PENDING</v>
       </c>
       <c r="G22" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H22" t="str">
         <v>April 24, 2025</v>
@@ -994,7 +994,7 @@
         <v>PENDING</v>
       </c>
       <c r="G23" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H23" t="str">
         <v>April 24, 2025</v>
@@ -1020,7 +1020,7 @@
         <v>PENDING</v>
       </c>
       <c r="G24" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H24" t="str">
         <v>April 24, 2025</v>
@@ -1046,7 +1046,7 @@
         <v>PENDING</v>
       </c>
       <c r="G25" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H25" t="str">
         <v>April 24, 2025</v>
@@ -1072,7 +1072,7 @@
         <v>PENDING</v>
       </c>
       <c r="G26" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H26" t="str">
         <v>April 24, 2025</v>
@@ -1098,7 +1098,7 @@
         <v>PENDING</v>
       </c>
       <c r="G27" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H27" t="str">
         <v>April 24, 2025</v>
@@ -1124,7 +1124,7 @@
         <v>PENDING</v>
       </c>
       <c r="G28" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H28" t="str">
         <v>April 24, 2025</v>
@@ -1150,7 +1150,7 @@
         <v>PENDING</v>
       </c>
       <c r="G29" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H29" t="str">
         <v>April 24, 2025</v>
@@ -1176,7 +1176,7 @@
         <v>PENDING</v>
       </c>
       <c r="G30" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H30" t="str">
         <v>April 24, 2025</v>
@@ -1202,7 +1202,7 @@
         <v>PENDING</v>
       </c>
       <c r="G31" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H31" t="str">
         <v>April 24, 2025</v>
@@ -1228,7 +1228,7 @@
         <v>PENDING</v>
       </c>
       <c r="G32" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H32" t="str">
         <v>April 24, 2025</v>
@@ -1254,7 +1254,7 @@
         <v>PENDING</v>
       </c>
       <c r="G33" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H33" t="str">
         <v>April 24, 2025</v>
@@ -1280,7 +1280,7 @@
         <v>PENDING</v>
       </c>
       <c r="G34" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H34" t="str">
         <v>April 24, 2025</v>
@@ -1306,7 +1306,7 @@
         <v>PENDING</v>
       </c>
       <c r="G35" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H35" t="str">
         <v>April 24, 2025</v>
@@ -1332,7 +1332,7 @@
         <v>PENDING</v>
       </c>
       <c r="G36" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H36" t="str">
         <v>April 24, 2025</v>
@@ -1358,7 +1358,7 @@
         <v>PENDING</v>
       </c>
       <c r="G37" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H37" t="str">
         <v>April 24, 2025</v>
@@ -1384,7 +1384,7 @@
         <v>PENDING</v>
       </c>
       <c r="G38" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H38" t="str">
         <v>April 24, 2025</v>
@@ -1410,7 +1410,7 @@
         <v>PENDING</v>
       </c>
       <c r="G39" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H39" t="str">
         <v>April 24, 2025</v>
@@ -1436,7 +1436,7 @@
         <v>PENDING</v>
       </c>
       <c r="G40" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H40" t="str">
         <v>April 24, 2025</v>
@@ -1462,7 +1462,7 @@
         <v>PENDING</v>
       </c>
       <c r="G41" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H41" t="str">
         <v>April 24, 2025</v>
@@ -1488,7 +1488,7 @@
         <v>PENDING</v>
       </c>
       <c r="G42" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H42" t="str">
         <v>April 24, 2025</v>
@@ -1618,7 +1618,7 @@
         <v>PENDING</v>
       </c>
       <c r="G47" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H47" t="str">
         <v>April 23, 2025</v>
@@ -1644,7 +1644,7 @@
         <v>PENDING</v>
       </c>
       <c r="G48" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H48" t="str">
         <v>April 23, 2025</v>
@@ -1670,7 +1670,7 @@
         <v>PENDING</v>
       </c>
       <c r="G49" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H49" t="str">
         <v>April 23, 2025</v>
@@ -1696,7 +1696,7 @@
         <v>PENDING</v>
       </c>
       <c r="G50" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H50" t="str">
         <v>April 23, 2025</v>
@@ -1722,7 +1722,7 @@
         <v>PENDING</v>
       </c>
       <c r="G51" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H51" t="str">
         <v>April 23, 2025</v>
@@ -1748,7 +1748,7 @@
         <v>PENDING</v>
       </c>
       <c r="G52" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H52" t="str">
         <v>April 23, 2025</v>
@@ -1774,7 +1774,7 @@
         <v>PENDING</v>
       </c>
       <c r="G53" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H53" t="str">
         <v>April 23, 2025</v>
@@ -1800,7 +1800,7 @@
         <v>PENDING</v>
       </c>
       <c r="G54" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H54" t="str">
         <v>April 23, 2025</v>
@@ -1826,7 +1826,7 @@
         <v>PENDING</v>
       </c>
       <c r="G55" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H55" t="str">
         <v>April 23, 2025</v>
@@ -1852,7 +1852,7 @@
         <v>PENDING</v>
       </c>
       <c r="G56" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H56" t="str">
         <v>April 23, 2025</v>
@@ -1878,7 +1878,7 @@
         <v>PENDING</v>
       </c>
       <c r="G57" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H57" t="str">
         <v>April 23, 2025</v>
@@ -1904,7 +1904,7 @@
         <v>PENDING</v>
       </c>
       <c r="G58" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H58" t="str">
         <v>April 23, 2025</v>
@@ -1930,7 +1930,7 @@
         <v>PENDING</v>
       </c>
       <c r="G59" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H59" t="str">
         <v>April 23, 2025</v>
@@ -1956,7 +1956,7 @@
         <v>PENDING</v>
       </c>
       <c r="G60" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H60" t="str">
         <v>April 23, 2025</v>
@@ -1982,7 +1982,7 @@
         <v>PENDING</v>
       </c>
       <c r="G61" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H61" t="str">
         <v>April 23, 2025</v>
@@ -2060,7 +2060,7 @@
         <v>PENDING</v>
       </c>
       <c r="G64" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H64" t="str">
         <v>April 22, 2025</v>
@@ -2086,7 +2086,7 @@
         <v>PENDING</v>
       </c>
       <c r="G65" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H65" t="str">
         <v>April 22, 2025</v>
@@ -2112,7 +2112,7 @@
         <v>PENDING</v>
       </c>
       <c r="G66" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H66" t="str">
         <v>April 22, 2025</v>
@@ -2138,7 +2138,7 @@
         <v>PENDING</v>
       </c>
       <c r="G67" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H67" t="str">
         <v>April 22, 2025</v>
@@ -2164,7 +2164,7 @@
         <v>PENDING</v>
       </c>
       <c r="G68" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H68" t="str">
         <v>April 22, 2025</v>
@@ -2190,7 +2190,7 @@
         <v>PENDING</v>
       </c>
       <c r="G69" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H69" t="str">
         <v>April 22, 2025</v>
@@ -2216,7 +2216,7 @@
         <v>PENDING</v>
       </c>
       <c r="G70" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H70" t="str">
         <v>April 22, 2025</v>
@@ -2242,7 +2242,7 @@
         <v>PENDING</v>
       </c>
       <c r="G71" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H71" t="str">
         <v>April 22, 2025</v>
@@ -2268,7 +2268,7 @@
         <v>PENDING</v>
       </c>
       <c r="G72" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H72" t="str">
         <v>April 22, 2025</v>
@@ -2294,7 +2294,7 @@
         <v>PENDING</v>
       </c>
       <c r="G73" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H73" t="str">
         <v>April 22, 2025</v>
@@ -2320,7 +2320,7 @@
         <v>PENDING</v>
       </c>
       <c r="G74" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H74" t="str">
         <v>April 22, 2025</v>
@@ -2346,7 +2346,7 @@
         <v>PENDING</v>
       </c>
       <c r="G75" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H75" t="str">
         <v>April 21, 2025</v>
@@ -2372,7 +2372,7 @@
         <v>PENDING</v>
       </c>
       <c r="G76" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H76" t="str">
         <v>April 21, 2025</v>
@@ -2398,7 +2398,7 @@
         <v>PENDING</v>
       </c>
       <c r="G77" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H77" t="str">
         <v>April 21, 2025</v>
@@ -2476,7 +2476,7 @@
         <v>PENDING</v>
       </c>
       <c r="G80" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H80" t="str">
         <v>April 21, 2025</v>
@@ -2502,7 +2502,7 @@
         <v>PENDING</v>
       </c>
       <c r="G81" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H81" t="str">
         <v>April 21, 2025</v>
@@ -2528,7 +2528,7 @@
         <v>PENDING</v>
       </c>
       <c r="G82" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H82" t="str">
         <v>April 20, 2025</v>
@@ -2580,7 +2580,7 @@
         <v>PENDING</v>
       </c>
       <c r="G84" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H84" t="str">
         <v>April 19, 2025</v>
@@ -2606,7 +2606,7 @@
         <v>PENDING</v>
       </c>
       <c r="G85" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H85" t="str">
         <v>April 19, 2025</v>
@@ -2658,7 +2658,7 @@
         <v>PENDING</v>
       </c>
       <c r="G87" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H87" t="str">
         <v>April 19, 2025</v>
@@ -2814,7 +2814,7 @@
         <v>PENDING</v>
       </c>
       <c r="G93" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H93" t="str">
         <v>April 18, 2025</v>
@@ -2840,7 +2840,7 @@
         <v>PENDING</v>
       </c>
       <c r="G94" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H94" t="str">
         <v>April 18, 2025</v>
@@ -2866,7 +2866,7 @@
         <v>PENDING</v>
       </c>
       <c r="G95" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H95" t="str">
         <v>April 18, 2025</v>
@@ -2918,7 +2918,7 @@
         <v>PENDING</v>
       </c>
       <c r="G97" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H97" t="str">
         <v>April 18, 2025</v>
@@ -2944,7 +2944,7 @@
         <v>PENDING</v>
       </c>
       <c r="G98" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H98" t="str">
         <v>April 18, 2025</v>
@@ -2996,7 +2996,7 @@
         <v>PENDING</v>
       </c>
       <c r="G100" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H100" t="str">
         <v>April 18, 2025</v>
@@ -3022,7 +3022,7 @@
         <v>PENDING</v>
       </c>
       <c r="G101" t="str">
-        <v>May 1, 2025</v>
+        <v>May 2, 2025</v>
       </c>
       <c r="H101" t="str">
         <v>April 18, 2025</v>

</xml_diff>